<commit_message>
add referral, treatment, diagnosis
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-mental-patient.xlsx
+++ b/output/StructureDefinition-mental-patient.xlsx
@@ -51,7 +51,7 @@
     <t>Status</t>
   </si>
   <si>
-    <t>active</t>
+    <t>draft</t>
   </si>
   <si>
     <t>Experimental</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-05-18T07:55:32+05:45</t>
+    <t>2025-05-20T08:23:51+05:45</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -4982,7 +4982,7 @@
         <v>91</v>
       </c>
       <c r="H26" t="s" s="2">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="I26" t="s" s="2">
         <v>83</v>

</xml_diff>